<commit_message>
fix the poor backlog
</commit_message>
<xml_diff>
--- a/docs/product backlog.xlsx
+++ b/docs/product backlog.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CodeArea\Software Engineering\EBU6304-2021-Software-Engineering-Group-111\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F123EF-0042-42FC-8AB4-B6BE2ED666C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="149">
   <si>
     <t>Story ID</t>
   </si>
@@ -433,7 +439,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>C</t>
     </r>
@@ -442,7 +448,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">heck card numbers </t>
     </r>
@@ -538,14 +544,6 @@
     <t>Configurable image printer</t>
   </si>
   <si>
-    <t xml:space="preserve">  As a   passenger      
-  I want my boarding check can come in picture form
-  So that  I can notice the important information easily.</t>
-  </si>
-  <si>
-    <t>-Verify that the image printer output is correct</t>
-  </si>
-  <si>
     <t>Check name of config entries</t>
   </si>
   <si>
@@ -554,10 +552,6 @@
   So that I can retrieve configuration.</t>
   </si>
   <si>
-    <t>-Verify that values can be check 
--Verify that names can be check</t>
-  </si>
-  <si>
     <t>Enhance the PaymentPanel textfield hint</t>
   </si>
   <si>
@@ -566,9 +560,6 @@
   So that they will  choose our airline next time.</t>
   </si>
   <si>
-    <t>-Verify the hint display logic is efficient</t>
-  </si>
-  <si>
     <t>Enhance the BillConfirmationPanel</t>
   </si>
   <si>
@@ -589,20 +580,35 @@
   </si>
   <si>
     <t>-Verify that every theme will be adapted in every panel.</t>
+  </si>
+  <si>
+    <t>-Verify the hint is hidden when and only when user clicks the text field</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>-Verify that only when names are complete can the software launch
+-Verify that only when values are complete can the software launch</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a   passenger      
+  I want my image printer is configurable
+  So that it can adapt to different physical printers</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>-Verify that the image printer can work on any physical printers once configed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,25 +620,17 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -640,147 +638,17 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,192 +657,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -997,256 +685,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1267,10 +716,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1292,61 +741,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="40% - 着色 1" xfId="1" builtinId="31"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1633,19 +1039,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
@@ -1659,7 +1065,7 @@
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="66" spans="1:9">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1121,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="66" spans="1:9">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1742,7 +1148,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="4" ht="93" spans="1:9">
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1769,7 +1175,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="5" ht="53" spans="1:9">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1202,7 @@
         <v>44649</v>
       </c>
     </row>
-    <row r="6" ht="108.6" customHeight="1" spans="1:9">
+    <row r="6" spans="1:9" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1823,7 +1229,7 @@
         <v>44640</v>
       </c>
     </row>
-    <row r="7" ht="53" spans="1:9">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1850,7 +1256,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="8" ht="93" spans="1:9">
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1877,7 +1283,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="9" ht="93" spans="1:9">
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1904,7 +1310,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="10" ht="66" spans="1:9">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1931,7 +1337,7 @@
         <v>44648</v>
       </c>
     </row>
-    <row r="11" ht="80" spans="1:9">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1958,7 +1364,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="12" ht="80" spans="1:9">
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1985,7 +1391,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="13" ht="80" spans="1:9">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1.4</v>
       </c>
@@ -2012,7 +1418,7 @@
         <v>44647</v>
       </c>
     </row>
-    <row r="14" ht="85.15" customHeight="1" spans="1:9">
+    <row r="14" spans="1:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -2039,7 +1445,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="15" ht="66" spans="1:9">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2.1</v>
       </c>
@@ -2066,9 +1472,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="16" ht="66" spans="1:9">
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>62</v>
@@ -2093,9 +1499,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="17" ht="66" spans="1:9">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>65</v>
@@ -2120,7 +1526,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="18" ht="53" spans="1:9">
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2.4</v>
       </c>
@@ -2147,7 +1553,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="19" ht="66" spans="1:9">
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>2.5</v>
       </c>
@@ -2174,7 +1580,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="20" ht="66" spans="1:9">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2.6</v>
       </c>
@@ -2201,7 +1607,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="21" ht="66" spans="1:9">
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3.1</v>
       </c>
@@ -2228,7 +1634,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="22" ht="66" spans="1:9">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3.2</v>
       </c>
@@ -2255,7 +1661,7 @@
         <v>44667</v>
       </c>
     </row>
-    <row r="23" ht="66" spans="1:9">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3.3</v>
       </c>
@@ -2282,7 +1688,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="24" ht="53" spans="1:9">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3.4</v>
       </c>
@@ -2309,7 +1715,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="25" ht="66" spans="1:9">
+    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>3.5</v>
       </c>
@@ -2336,7 +1742,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="26" ht="66" spans="1:9">
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>3.6</v>
       </c>
@@ -2363,7 +1769,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="27" ht="66" customHeight="1" spans="1:9">
+    <row r="27" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>3.7</v>
       </c>
@@ -2390,7 +1796,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="28" ht="80" spans="1:9">
+    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3.8</v>
       </c>
@@ -2417,7 +1823,7 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="29" ht="53" spans="1:9">
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>3.9</v>
       </c>
@@ -2444,7 +1850,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="30" ht="66" spans="1:9">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>3.1</v>
       </c>
@@ -2471,9 +1877,9 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="31" ht="66" spans="1:9">
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>107</v>
@@ -2498,7 +1904,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="32" ht="53" spans="1:9">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>4.2</v>
       </c>
@@ -2525,7 +1931,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="33" ht="66" spans="1:9">
+    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>4.3</v>
       </c>
@@ -2552,9 +1958,9 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="34" ht="80" spans="1:9">
+    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>116</v>
@@ -2579,7 +1985,7 @@
         <v>44688</v>
       </c>
     </row>
-    <row r="35" ht="66" spans="1:9">
+    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>4.5</v>
       </c>
@@ -2606,9 +2012,9 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="36" ht="53" spans="1:9">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>122</v>
@@ -2633,7 +2039,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="37" ht="53" spans="1:9">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>4.7</v>
       </c>
@@ -2660,7 +2066,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="38" ht="53" spans="1:9">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4.8</v>
       </c>
@@ -2687,9 +2093,9 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="39" ht="53" spans="1:9">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>131</v>
@@ -2714,7 +2120,7 @@
         <v>44699</v>
       </c>
     </row>
-    <row r="40" ht="66" spans="1:9">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>5.2</v>
       </c>
@@ -2722,7 +2128,7 @@
         <v>134</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D40" s="5">
         <v>2</v>
@@ -2731,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="14">
@@ -2741,15 +2147,15 @@
         <v>44702</v>
       </c>
     </row>
-    <row r="41" ht="53" spans="1:9">
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>5.3</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D41" s="5">
         <v>2</v>
@@ -2758,7 +2164,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="14">
@@ -2768,15 +2174,15 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="42" ht="80" spans="1:9">
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>5.4</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D42" s="5">
         <v>4</v>
@@ -2785,7 +2191,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="14">
@@ -2795,15 +2201,15 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="43" ht="53" spans="1:9">
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>5.5</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D43" s="5">
         <v>4</v>
@@ -2812,7 +2218,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="14">
@@ -2822,15 +2228,15 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="44" ht="66" spans="1:9">
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>5.6</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D44" s="5">
         <v>5</v>
@@ -2839,7 +2245,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="14">
@@ -2849,24 +2255,24 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="45" spans="9:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="9:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="9:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="9:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I48" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I28">
     <sortCondition ref="D2"/>
   </sortState>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <headerFooter/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amend backlog 5.1 and 5.5
</commit_message>
<xml_diff>
--- a/docs/product backlog.xlsx
+++ b/docs/product backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CodeArea\Software Engineering\EBU6304-2021-Software-Engineering-Group-111\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EBU6304-2021-Software-Engineering-Group-111\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F123EF-0042-42FC-8AB4-B6BE2ED666C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F837BE-C3C0-47D8-9240-AD763EFC891A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,15 +532,6 @@
     <t>Enhance the FlightInfoCard</t>
   </si>
   <si>
-    <t xml:space="preserve">  As a  passenger,
-  I want to know whether the flight will span several days,
-  So that I better travel plan.</t>
-  </si>
-  <si>
-    <t>-Verify that the date and time shown are correct
--Verify that the layout is concise and beautiful</t>
-  </si>
-  <si>
     <t>Configurable image printer</t>
   </si>
   <si>
@@ -563,20 +554,7 @@
     <t>Enhance the BillConfirmationPanel</t>
   </si>
   <si>
-    <t xml:space="preserve">  As an airline staff        
-  I want to have a better looking system
-  So that   customers will get more information on one page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-Verify that the layout and font are beautiful and practical </t>
-  </si>
-  <si>
     <t>Update the theme libarary</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As an airline staff
-  I want my customer could have more theme to choose 
-  So that  they could have better flying experience.</t>
   </si>
   <si>
     <t>-Verify that every theme will be adapted in every panel.</t>
@@ -598,6 +576,34 @@
   </si>
   <si>
     <t>-Verify that the image printer can work on any physical printers once configed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a  passenger,
+  I want to know whether the flight will span several days,
+  So that I can know better about the time of flight.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>-Verify that the time span shows correctly
+-Verify that the time span label is concealed if the flight time is less that 24 hours.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> As an airline staff
+  I want my customer could have more theme to choose 
+  So that  they could have better flying experience.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a passenger      
+  I want to get more information about the flight I'm checking in
+  So that I would confirm my check-in with more confidence.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>-Verify that the information on the passport is precisely aligned with the background image.
+-Verify that 2 bill cards' sizes will not be affected by number of preferences selected.</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -606,7 +612,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -716,7 +722,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1047,21 +1053,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="21.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1094,7 +1100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>44640</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1283,7 +1289,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>44648</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1.4</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>44647</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="85.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2.1</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -1499,7 +1505,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2.4</v>
       </c>
@@ -1553,7 +1559,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>2.5</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2.6</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3.1</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3.2</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>44667</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3.3</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3.4</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>3.5</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>3.6</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3.8</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>3.9</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>3.1</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>4.2</v>
       </c>
@@ -1931,7 +1937,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>4.3</v>
       </c>
@@ -1958,7 +1964,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>44688</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>4.5</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>4.7</v>
       </c>
@@ -2066,7 +2072,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4.8</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>5.0999999999999996</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="D39" s="5">
         <v>1</v>
@@ -2110,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="14">
@@ -2120,15 +2126,15 @@
         <v>44699</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>5.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D40" s="5">
         <v>2</v>
@@ -2137,7 +2143,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="14">
@@ -2147,15 +2153,15 @@
         <v>44702</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>5.3</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" s="5">
         <v>2</v>
@@ -2164,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="14">
@@ -2174,15 +2180,15 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>5.4</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D42" s="5">
         <v>4</v>
@@ -2191,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="14">
@@ -2201,15 +2207,15 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>5.5</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D43" s="5">
         <v>4</v>
@@ -2218,7 +2224,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="14">
@@ -2228,15 +2234,15 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>5.6</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D44" s="5">
         <v>5</v>
@@ -2245,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="14">

</xml_diff>